<commit_message>
lagou http request optimize
</commit_message>
<xml_diff>
--- a/output/lagou.xlsx
+++ b/output/lagou.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
+  <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
     <s:workbookView activeTab="0"/>
   </s:bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>corp_name</t>
   </si>
@@ -41,13 +41,141 @@
     <t>corp_products</t>
   </si>
   <si>
-    <t>阿里巴巴</t>
-  </si>
-  <si>
-    <t>淘宝（中国）软件有限公司</t>
-  </si>
-  <si>
-    <t>电子商务,生活服务</t>
+    <t>爱车阵</t>
+  </si>
+  <si>
+    <t>好卡（北京）网络技术有限公司</t>
+  </si>
+  <si>
+    <t>移动互联网</t>
+  </si>
+  <si>
+    <t>天使轮</t>
+  </si>
+  <si>
+    <t>少于15人</t>
+  </si>
+  <si>
+    <t>北京</t>
+  </si>
+  <si>
+    <t>我们是一家Startup（初创）公司，有雅虎，阿里，美团等互联网人士创立，致力与服务中国1.3亿的汽车消费人群，打造中国的AAA。
+我们的愿景：
+ 1、省钱省心、以车会友；
+ 2、让每个车主都有一个自己喜欢的车友会
+我们的产品观：一个好的产品不是靠单纯的创新，而是基于对目标群体深度的、细腻的需求的理解，解决他们问题的同时，带来超乎想象的体验。 
+关于团队：核心团队来自雅虎，阿里巴巴，美团等，有超过10年以上者名互联网从业的老兵们，也有19岁的技术极客，有二次创业永不言败的战士，也有BAT技术大牛，既有单身的帅哥美女，也有24小时不分离的准夫妻共事一堂， 既有国际知名学府的人才，也能接纳自学成才的牛人，这里没有等级阶层，只有创业伙伴， 来吧，就等你了。
+我们的优势：磨合里两年多的激情团队，不离不弃的汽车方向，全国上千车友会联盟，独特的产品定位；
+投资和荣誉：
+1、真格基金天使基金
+2、华创Pre-A投资
+3、中关村雏鹰人才计划成员企业。</t>
+  </si>
+  <si>
+    <t>天翼科技创业投资有限公司</t>
+  </si>
+  <si>
+    <t>未融资</t>
+  </si>
+  <si>
+    <t>15-50人</t>
+  </si>
+  <si>
+    <t>上海</t>
+  </si>
+  <si>
+    <t>中国电信天翼科技创业投资有限公司（中国电信创新孵化基地）是中国电信集团主业范围内的全资一级子公司，是中国电信实施战略转型、推进科技创新的重要战略单元。
+    公司位于上海市浦东新区杨高南路5678弄中国电信信息园区内。公司聚焦移动互联网、云计算和物联网等战略性新兴业务，坚持“专业孵化+创业导师+天使投资”的孵化模式，将中国电信的资金、网络、技术、人才、创意等资源与社会科技创新环境及资本进行高效整合对接，积极扶持内部员工和社会有志之士的早期创业。公司在立足资源和品牌优势的同时，积极引入民企的股权和人才激励机制，同时开放社会资本参与渠道，打造国内领先的创业服务和投融资平台。
+公司力争在信息产业领域培育一批龙头企业，培养一批企业家和创新人才，打造规模化、体系化、高端化的信息产业集群，有效推动科技创新企业的聚集与发展，开创国有资本体系下推动自主创新和企业发展的新模式。</t>
+  </si>
+  <si>
+    <t>和创业者一起成就梦想,</t>
+  </si>
+  <si>
+    <t>上海奕行</t>
+  </si>
+  <si>
+    <t>上海奕行信息科技公司</t>
+  </si>
+  <si>
+    <t>文化娱乐</t>
+  </si>
+  <si>
+    <t>上海奕行公司核心创业人员主要来自于中国电信全球眼研发团队，基于安防视频监控技术，进行视频的聚合/转换/分发/分析等处理，形成智能交通实时路况信息，为车联网等企业和个人用户提供实景路况服务，开发智慧旅游景区实景展示方案。公司由中国电信天翼创投进行投资，与中国电信等运营商有密切的合作关系。</t>
+  </si>
+  <si>
+    <t>翼行</t>
+  </si>
+  <si>
+    <t>百付天下</t>
+  </si>
+  <si>
+    <t>上海翰鑫信息科技有限公司</t>
+  </si>
+  <si>
+    <t>B轮</t>
+  </si>
+  <si>
+    <t>50-150人</t>
+  </si>
+  <si>
+    <t>上海翰鑫信息科技有限公司（以下简称翰鑫科技）成立于2010年9月，正值移动互联网步入发展阶段，市场氛围及用户认知度也相当良好，为翰鑫科技的发展提供了良好的环境！
+ 目前是中国银联的战略合作伙伴。同时，翰鑫科技与三大运营商及保险、商旅、航空等机构建立了良好的合作关系。
+ 翰鑫科技的移动支付产品系列已从原来的单一“智能卡支付”扩展到手机应用内支付、WAP支付、IVR语音支付、微支付、SMS支付等多款产品。同时，为运维着多个业务平台，包括：资金归集平台、信用卡还款转账平台、O2O无卡消费平台等。并在此基础之上，为行业客户提供整体解决方案。
+ 公司从原有的十几个人扩展到目前的140多名正式员工，并且拥有上海总部、北京、江苏、浙江多个分支业务机构。为翰鑫科技的长足发展奠定了扎实的技术、业务基础。</t>
+  </si>
+  <si>
+    <t>唯医网</t>
+  </si>
+  <si>
+    <t>北京欧应科技有限公司</t>
+  </si>
+  <si>
+    <t>150-500人</t>
+  </si>
+  <si>
+    <t>北京欧应科技有限公司是一家专注于专业医疗教育的垂直社交类的专业网站，拥有国内外众多高端的医疗教育资源，通过先进高效的网络技术（如视频互动直播），为专业的医疗人员提供及时、全面、互动、分享的医学专业信息和知识分享的平台，同时开展线下专业教育与培训活动。本公司为医疗与互联网技术整合的领导者，并推动着行业的快速发展。</t>
+  </si>
+  <si>
+    <t>唯医</t>
+  </si>
+  <si>
+    <t>北京鼎天</t>
+  </si>
+  <si>
+    <t>北京鼎天投资管理有限公司</t>
+  </si>
+  <si>
+    <t>金融</t>
+  </si>
+  <si>
+    <t>北京鼎天投资管理有限公司是一家集资产管理、投资于一身的集团化企业，总部设在北京CBD核心区。在香港和上海有分支机构。主营业务为股权投资及证券投资，对冲基金及衍生产品投资等。公司将秉承开放、创新、诚信、共荣的原则，以信息及人才为优势，立足长远，建设成为具备一流规模和影响力的资产管理公司。现诚邀行业精英加盟，共享广阔前景。</t>
+  </si>
+  <si>
+    <t>优米网</t>
+  </si>
+  <si>
+    <t>北京优视米网络科技有限公司</t>
+  </si>
+  <si>
+    <t>教育,文化娱乐</t>
+  </si>
+  <si>
+    <t>北京优视米网络科技有限公司成立于2010年3月17日，是由著名制片人王利芬女士创办，经国家广播电影电视总局批准拥有视频节目制作权和视频试听许可证的民营机构。
+ 优米公司面向创业者提供多维度的服务，优米网是公司旗下的视频网站，是为创业者提供有价值视频的服务平台。视频产品聚焦“创业”智慧，提供在线点播等服务，是“创业智慧供应商”。优米网同时为手机用户打造优质的移动客户端创业课件。
+优米网自制视频团队拥有一流的策划制作能力，曾制作《赢在中国》、《我们》、《在路上》等知名栏目。</t>
+  </si>
+  <si>
+    <t>创业实操课程</t>
+  </si>
+  <si>
+    <t>聚美优品</t>
+  </si>
+  <si>
+    <t>北京创锐文化传媒有限公司</t>
+  </si>
+  <si>
+    <t>电子商务</t>
   </si>
   <si>
     <t>上市公司</t>
@@ -56,24 +184,59 @@
     <t>2000人以上</t>
   </si>
   <si>
-    <t>北京</t>
-  </si>
-  <si>
-    <t xml:space="preserve">阿里巴巴网络技术有限公司（简称：阿里巴巴集团）是以曾担任英语教师的
-马云为首的18人，于1999年在中国杭州创立，他们相信互联网能够创造公平的竞争环境，让小企业通过创新与科技扩展业务，并在参与国内或全球市场竞争时处于更有利的位置。[1]
- 阿里巴巴集团经营多项业务，另外也从关联公司的业务和服务中取得经营商业生态系统上的支援。业务和关联公司的业务包括：
-淘宝网、
-天猫、
-聚划算、
-全球速卖通、阿里巴巴国际交易市场、
-1688、
-阿里妈妈、
-阿里云、
-蚂蚁金服、
-菜鸟网络等。[2]
- 2014年9月19日，阿里巴巴集团在纽约证券交易所正式挂牌上市，股票代码“BABA”，创始人和董事局主席为
-马云。2015年全年，阿里巴巴总营收943.84亿元人民币，净利润688.44亿元人民币。
+    <t>聚美优品中国最大的化妆品限时特卖商城，由海归学子陈欧、戴雨森创立于2010年3月，致力于创造简单、有趣、值得信赖的化妆品购物体验。
+ 2014年5月，聚美优品作为中国最大的美妆电商，登陆美国纽约证券交易所挂牌上市，成为近年中国发展速度最快的电子商务公司之一。
+发展至今
+聚美优品注册用户数量突破千万级、月销售超过6亿元、品牌官方授权商品最多，是唯一拥有防伪码体系，能够实现化妆品官网验真的电商。
+先后在天津、上海、广州、成都、沈阳、郑州等地建立总面积达六七万平米的自建仓储、保税仓，并布局香港、日韩、欧美等海外市场，领跑化妆品海外购市场，每天将全球最新潮、火爆、好用的商品搬到用户手机上。
+全方位打造简单、有趣、值得信赖的化妆品购物体验。</t>
+  </si>
+  <si>
+    <t>瓦力</t>
+  </si>
+  <si>
+    <t>北京瓦力网络科技有限公司</t>
+  </si>
+  <si>
+    <t>A轮</t>
+  </si>
+  <si>
+    <t>瓦力是一家致力于无线互联网技术开发及应用服务的专业技术型企业。公司专注于精品游戏平台的运营，是国内知名的游戏运营平台——小米游戏中心的开发商和运营服务提供商。目前，我们的业务不仅仅只限于手机游戏，小米盒子、小米电视，这些小米最发烧的配件都内置有我们的游戏中心。你的工作成果将不断的在最具充满想象空间的智能设备上体现。</t>
+  </si>
+  <si>
+    <t>小米游戏平台的运营</t>
+  </si>
+  <si>
+    <t>今日头条</t>
+  </si>
+  <si>
+    <t>北京字节跳动科技有限公司</t>
+  </si>
+  <si>
+    <t>移动互联网,数据服务</t>
+  </si>
+  <si>
+    <t>C轮</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    “今日头条”是一款基于数据挖掘的推荐引擎产品，是国内移动互联网领域成长最快的产品服务之一。“今日头条”第一个版本于2012年8月上线，截至2016年9月，“今日头条”已经在为超过5.5亿的忠诚用户服务，每天有超过6000万的用户在头条上找到让他们了解世界、启发思考、开怀一笑的信息，并活跃地参与互动。 
+    “今日头条”的团队是一支拥有丰富创业及成熟公司经验的靠谱团队，聚集了来自一流学校和一流公司的顶尖人才，在推荐引擎、机器学习等技术领域拥有与世界级公司接轨的能力。公司正处于高速发展期，2014年6月，今日头条获得C轮1亿美元的融资。
+      我们崇尚简单，始终关注用户需求，热衷于把从用户界面上的每一个细节体验到后台的海量数据处理都做到极致；我们推崇在轻松，快乐的环境中学习，积累，分享和成长。在这里，我们每天都在创造价值，产生影响。
 </t>
+  </si>
+  <si>
+    <t>先智创科</t>
+  </si>
+  <si>
+    <t>先智创科（北京）科技有限公司</t>
+  </si>
+  <si>
+    <t>先智创科，2011年成立于北京，是一家技术型互联网公司，主要从事金融用户数据挖掘和金融产品网络营销业务。公司运营两年以来，为阳光保险、大地保险、渣打银行等多十家金融机构，提供过用户数据分析与价值挖掘，以及产品营销与品牌推广服务。
+对于金融消费者，先智创科通过旗下91金融超市、贷乐发、易贷天下等工具型金融媒体，为金融产品消费者和金融机构搭建的一个信息平台。在这里，贷款、保险、车险、证券、基金等等，凡是能想到的金融产品都有一席之地，金融消费者可以解决同类金融服务机构的价格、服务比较问题，找到最优惠的购买渠道。不只是通过互联网访问，还可以通过手机APP直接在手机上完成操作，或者通过微博、微信等社交网络完成消费，或者直接拨打400-000-9335免费客服电话直接完成。
+对于金融机构，先智创科按照保险、银行等不同行业客户的需求，提供定制化的数据及营销服务。金融机构或其从业人员，可以通过互联网或者手机，直接找到符合其产品定位并且有购买意向的消费者。目前，跨多个平台的用户日均流量达到300,000 UV，单个消费者的成单周期一般在1-3天，而平均每个金融服务机构日接单量能够达到100单。</t>
+  </si>
+  <si>
+    <t>91金融-贷乐发,91金融-易贷天下,91金融-车险通</t>
   </si>
 </sst>
 </file>
@@ -410,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,30 +607,323 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="15" spans="1:9">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E15" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G15" t="s">
         <v>13</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H15" t="s">
         <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>28</v>
+      </c>
+      <c r="F44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+      <c r="H50" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I54" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" t="s">
+        <v>29</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>54</v>
+      </c>
+      <c r="I59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" t="s">
+        <v>57</v>
+      </c>
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" t="s">
+        <v>49</v>
+      </c>
+      <c r="G63" t="s">
+        <v>13</v>
+      </c>
+      <c r="H63" t="s">
+        <v>60</v>
+      </c>
+      <c r="I63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" t="s">
+        <v>62</v>
+      </c>
+      <c r="D65" t="s">
+        <v>47</v>
+      </c>
+      <c r="E65" t="s">
+        <v>28</v>
+      </c>
+      <c r="F65" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" t="s">
+        <v>63</v>
+      </c>
+      <c r="I65" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>